<commit_message>
Update 2022 tower spreadsheet
</commit_message>
<xml_diff>
--- a/data/tower_count/tower_count_2022.xlsx
+++ b/data/tower_count/tower_count_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejgna\Documents\project-eleanor-and-wriley\data\tower_count\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8D77DEC-791A-44C3-BDE4-B9540161FEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4953430B-F2E0-461D-8A05-A29A53DDE5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{2C4A9B33-4602-4668-A628-2701EBBE869D}"/>
   </bookViews>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC6FB5A4-9062-4F33-A791-0909C7DC95E4}">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>